<commit_message>
[MCP-203] Changes per Harish's new PR.
</commit_message>
<xml_diff>
--- a/sample-data/7110_aortic-aneurysm.xlsx
+++ b/sample-data/7110_aortic-aneurysm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/mapped_docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Odin\workspace\mcp-data-client\sample-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD816EB-6369-AA40-8DBD-9EE0238B7F68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F79ADB-CA9F-489F-8837-19D2D3D67C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1260" yWindow="-19160" windowWidth="33600" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Eval Builder Calculator: aortic-aneurysm</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Symptomatic</t>
-  </si>
-  <si>
-    <t>DBQ8035_175 AND DBQ8035_177</t>
   </si>
   <si>
     <t>DBQ8035_175 AND DBQ8035_181</t>
@@ -119,7 +116,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,20 +489,22 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -534,7 +533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="32">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -550,14 +549,11 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="32">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -574,13 +570,13 @@
         <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="80">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -597,19 +593,19 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="6" spans="1:10" ht="128">
+    <row r="6" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -626,19 +622,19 @@
         <v>20</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="32">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -655,7 +651,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -667,6 +663,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED79F0EC3E5F7247B5468DE2217405EE" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b0145cebf11610b3540f9df2faf3a333">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71f3003f-14ae-4fd3-ad87-6fa34bd771ad" xmlns:ns3="bf4ccbb4-a8ef-483a-aefe-5e3e6c720a8e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0ffa6e98728e15f31cc3911c2059b17" ns2:_="" ns3:_="">
     <xsd:import namespace="71f3003f-14ae-4fd3-ad87-6fa34bd771ad"/>
@@ -883,7 +885,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -892,20 +894,38 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B58284F-0F3F-499A-B641-9E0E3BC5832B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{287C4334-6A1E-4759-B264-0453B43418FF}"/>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{287C4334-6A1E-4759-B264-0453B43418FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71f3003f-14ae-4fd3-ad87-6fa34bd771ad"/>
+    <ds:schemaRef ds:uri="bf4ccbb4-a8ef-483a-aefe-5e3e6c720a8e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2071D6F2-9512-4562-AC88-8924956E1C0E}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B58284F-0F3F-499A-B641-9E0E3BC5832B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2071D6F2-9512-4562-AC88-8924956E1C0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>